<commit_message>
Updated timesheet-Sheik & Darshana
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A37DAE1A-BBEA-4E6A-8AFF-172D42D8D5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FECBBC4B-91A8-4C27-B311-FA516FF4C590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="188">
   <si>
     <t>Column1</t>
   </si>
@@ -723,8 +723,18 @@
 </t>
   </si>
   <si>
+    <t>Dependencies for theTAC and Admin</t>
+  </si>
+  <si>
     <t xml:space="preserve">8:45-9:00 - Brainstorming with team
-9:00-10:00 - Designed Layout for HomePage
+9:00-10:30 - Created Architecture diagram in entity level for TAC and Admin
+10:30-10:50 -Break
+11:00-12:20 - Created Architecture diagram in Service level for TAC and Admin
+12:20-12:45 - Created HLD document                                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:45-9:00 - Brainstorming with team
+9:00-10:00 - Referred Bootstrap and designed common layout 
 10:15-10:50 - Proxy Pattern session with Rafi
 10:50-11:00 - Break
 11:00-12:10 - Designing Layout for Dashboard </t>
@@ -733,7 +743,17 @@
     <t>40mins</t>
   </si>
   <si>
-    <t xml:space="preserve">Seeking for more NFR and Pain points. </t>
+    <t>Dependencies for the 2 Users (Interviewer, Management)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:45-9:00 - Brainstorming 
+9:00-10:30 - Created Architecture diagram in entity level for interviewer and management.
+10:30-10:50 -Break
+11:00-12:20 - Created Architecture diagram in Service level for interviewer and management.
+12:20-12:45 - Created HLD document                                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seeking for more NFR and Pain points, Interactions. </t>
   </si>
   <si>
     <t xml:space="preserve">8.45 am - 9.00 am : Discussion with team mates.
@@ -8297,8 +8317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164F129C-4B66-4886-90DA-03408C042996}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8423,19 +8443,19 @@
         <v>17</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>165</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>166</v>
+        <v>180</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>181</v>
       </c>
       <c r="E9" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F9" s="35">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="G9" s="35">
-        <v>1.2</v>
+        <v>0.2</v>
       </c>
       <c r="H9" s="24"/>
     </row>
@@ -8447,7 +8467,7 @@
         <v>167</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E10" s="35" t="s">
         <v>41</v>
@@ -8456,7 +8476,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H10" s="24"/>
     </row>
@@ -8545,19 +8565,19 @@
         <v>31</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>158</v>
+        <v>184</v>
       </c>
       <c r="D15" s="47" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F15" s="45">
-        <v>2.5</v>
+        <v>3.2</v>
       </c>
       <c r="G15" s="35">
-        <v>1.2</v>
+        <v>0.2</v>
       </c>
       <c r="H15" s="26"/>
     </row>
@@ -8585,10 +8605,10 @@
         <v>54</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Updated Timesheet nd API -Prithvi
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DCF4F85-0F49-4ED2-B213-894E273967AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32FE14C4-A086-453E-A390-BC722C6874A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="12" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="12" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 3(06-04-2022)" sheetId="40" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="230">
   <si>
     <t>Column1</t>
   </si>
@@ -931,10 +931,10 @@
     <t xml:space="preserve">                                                      Have to work on Api Implementations</t>
   </si>
   <si>
-    <t>9:30am to 10:00am : Brainstorming with team    
+    <t xml:space="preserve">9:30am to 10:00am : Brainstorming with team    
 10.10am to 11.30 am : Implemented Role Service and Role Model for API
 12.00pm to 12.30pm : Worked on EF Code First for Role Model class 
-12.30pm to 1.00 : System Allocation.</t>
+12.30pm to 1.00 : System Allocation.                                1.45pm to 3.00pm : worked on Data Acess layer            3.30pm to 4.15pm : Meeting with Rafi(changes in Operations and Api ) </t>
   </si>
   <si>
     <t xml:space="preserve"> 9:30 to 10:00 -Brainstorming with team                             10:00 to 10:30 - Working on layout for TAC's Upcoming drive.                                                                                          10:30 to 11:30 - Session with rafi.                                        11:30 to 11:45 - Break                                                           11:45 to 12:30 - continued on desiging the upcoming drives page .</t>
@@ -950,6 +950,15 @@
     <t>9:30am to 10:00am : Brainstorming with team    
 10.30am to 12.30 am : Reviewed Data model
 12.30pm to 1.00 : System Allocation</t>
+  </si>
+  <si>
+    <t>Have to work on Api Implementations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.45am to 9.15am : worked on data acess layer for api
+9.15am to 10.30  : worked on Data Factory Classes
+10.30am to 10.45 : Refered sample API code in GitHub
+11.15am to 12.45 : worked on exception handling for api.                                                                                              1.30pm to 2.00 : reviewed my api implementation </t>
   </si>
   <si>
     <t>8.45 to 9.00 - Updating MOM &amp; Checking Mail
@@ -10830,8 +10839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FFC9C9-2848-4E62-84AF-44A9BCE5AD3F}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11147,8 +11156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7B8EE2-C09E-4672-919D-0F2EB56C51A0}">
   <dimension ref="A4:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11352,10 +11361,10 @@
         <v>27</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="D15" s="44" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
@@ -11397,7 +11406,7 @@
         <v>224</v>
       </c>
       <c r="D17" s="47" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Updated TimeSheet and Services
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32FE14C4-A086-453E-A390-BC722C6874A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0EDC525-F3D5-45F7-99BD-1EAA4C8A13FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="12" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="13" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 3(06-04-2022)" sheetId="40" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="232">
   <si>
     <t>Column1</t>
   </si>
@@ -947,9 +947,9 @@
 11.15to 11.45-Break                                                                11.45 to 12.30 - Studied how to connect EF with Web API Project                                                                               1.00 to 2.00 - Lunch                                                                     2.00 to 3.00 - How to use Postman App ( get post put methods, Using api's )                                                                     3.00 to 3.30 -  Idle                                                                                      3.30 to 4.00 - Review Meeting with Rafi                                                                </t>
   </si>
   <si>
-    <t>9:30am to 10:00am : Brainstorming with team    
+    <t xml:space="preserve">9:30am to 10:00am : Brainstorming with team    
 10.30am to 12.30 am : Reviewed Data model
-12.30pm to 1.00 : System Allocation</t>
+12.30pm to 1.00 am: System Allocation                           1.45 pm - 3.15 pm : Refined services                            3.30 pm - 4.10  pm: review with rafi(data model, WebApi, layout) </t>
   </si>
   <si>
     <t>Have to work on Api Implementations</t>
@@ -967,6 +967,14 @@
 10.45 to 11.15 - Break
 11.15 to 11.30 - General team Discussion
 11.30 to 12.30 - Created prototype for Admin ( final version )</t>
+  </si>
+  <si>
+    <t>Working on Register screen</t>
+  </si>
+  <si>
+    <t>8.45 am - 10.45 am : Corrections done in Data model and Prototype
+11.15 am - 12.45 pm : register layout
+1.15 pm - 2.30 pm : Refined Services(Role, Department, Employee, Drive, Pool, Location)</t>
   </si>
 </sst>
 </file>
@@ -10839,8 +10847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FFC9C9-2848-4E62-84AF-44A9BCE5AD3F}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11054,7 +11062,7 @@
         <v>41</v>
       </c>
       <c r="F13" s="35">
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="G13" s="35">
         <v>0</v>
@@ -11115,7 +11123,7 @@
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="35">
-        <v>2.5</v>
+        <v>6.5</v>
       </c>
       <c r="G16" s="35">
         <v>0</v>
@@ -11156,8 +11164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7B8EE2-C09E-4672-919D-0F2EB56C51A0}">
   <dimension ref="A4:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11370,7 +11378,7 @@
         <v>41</v>
       </c>
       <c r="F15" s="35">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="G15" s="35">
         <v>0</v>
@@ -11424,12 +11432,14 @@
         <v>34</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="D18" s="44"/>
+        <v>230</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>231</v>
+      </c>
       <c r="E18" s="35"/>
       <c r="F18" s="35">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="G18" s="35">
         <v>0</v>

</xml_diff>

<commit_message>
Updated time sheet - Sheik Fareeth H, Remuki, Gokul
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25216"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25217"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B05547DA-F93C-4E5B-9F79-FAA005AEA20B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2598BE30-3BFA-401B-9491-14E8AE006B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="13" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 3(06-04-2022)" sheetId="40" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="252">
   <si>
     <t>Column1</t>
   </si>
@@ -1098,6 +1098,48 @@
 9:45-10:45- Softskills Session with Savitha(about Problem Solving)
 10:45-11:00 - Break
 11:00-12:00 - Corrected Layout page for Profile</t>
+  </si>
+  <si>
+    <t>Today :
+8.45-9.30Am System allocation and installation
+9.30-10.30Am Sessin with Savitha
+10.30-10.45Am Break
+10.45-12.00Am Layout for Create Invite
+Yesterday :
+4.20 to 4.40 : Estimation session with Rafi
+4.45-5.30Pm college project meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Yesterday :
+1:30 to 2:30    - lunch
+3:00 to 3:45    - Review meeting with Raafi.
+3:45 to 4:10    - Break.
+4:10 to 4:20    - Idle 
+4:20 to 4:40    - Estimation session with Raafi.
+4:40 to 6:00    - Worked on upcoming drives page.                                 Today:
+8:45 to 9:00      - Checked in the mail.
+9:00 to 9:30      - Working on listing page.
+9:30 to 10:30     - Softskills session with savitha ( Problem solving).
+10:30 to 10:45    - Break
+10:45 to 12:30    - continued on listing (pagination,responsiveness).</t>
+  </si>
+  <si>
+    <t>Yesterday :
+1.30 to 2.30 : lunch
+3.00 to 3.45 : Review Meeting with Rafi
+3.45 to 4.10 : Break
+4.20 to 4.40 : Estimation session with Rafi
+4.40 to 5.45 : Wroked on unique page identification for the whole system.
+5.45 to 6.00 : General team meeting on Layouts &amp; Unique pages in the system
+Today :
+8.45 to 9.00 : Checking mails &amp; Filled bank details for Pay role
+9.00 to 9.15 : Updating MOM
+9.15 to 9.30 : Surfed how to publish HTML pages in Github
+9.45 to 10.30 : Soft skill session with Savitha.
+10.30 to 11.00 : Break
+11.00 to 12.00 : Identifying unique pages and Operations for Estimation
+12.00 to 1.00 : Listing down the API usage for particular pages for reuse and Estimation</t>
   </si>
 </sst>
 </file>
@@ -12162,8 +12204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7B8EE2-C09E-4672-919D-0F2EB56C51A0}">
   <dimension ref="A4:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12282,7 +12324,7 @@
       </c>
       <c r="H10" s="23"/>
     </row>
-    <row r="11" spans="1:8" ht="315" customHeight="1">
+    <row r="11" spans="1:8" ht="348" customHeight="1">
       <c r="B11" s="19" t="s">
         <v>17</v>
       </c>
@@ -12303,7 +12345,7 @@
       </c>
       <c r="H11" s="24"/>
     </row>
-    <row r="12" spans="1:8" ht="287.25" customHeight="1">
+    <row r="12" spans="1:8" ht="327.75" customHeight="1">
       <c r="B12" s="19" t="s">
         <v>20</v>
       </c>
@@ -12324,7 +12366,7 @@
       </c>
       <c r="H12" s="24"/>
     </row>
-    <row r="13" spans="1:8" ht="186.75" customHeight="1">
+    <row r="13" spans="1:8" ht="230.25" customHeight="1">
       <c r="B13" s="19" t="s">
         <v>21</v>
       </c>
@@ -12332,7 +12374,7 @@
         <v>233</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>41</v>
@@ -12362,7 +12404,7 @@
       <c r="G14" s="35"/>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="211.5" customHeight="1">
+    <row r="15" spans="1:8" ht="178.5" customHeight="1">
       <c r="B15" s="19" t="s">
         <v>27</v>
       </c>
@@ -12383,7 +12425,7 @@
       </c>
       <c r="H15" s="25"/>
     </row>
-    <row r="16" spans="1:8" ht="204" customHeight="1">
+    <row r="16" spans="1:8" ht="395.25" customHeight="1">
       <c r="B16" s="19" t="s">
         <v>30</v>
       </c>
@@ -12391,7 +12433,7 @@
         <v>167</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>41</v>
@@ -12404,7 +12446,7 @@
       </c>
       <c r="H16" s="25"/>
     </row>
-    <row r="17" spans="2:8" ht="232.5" customHeight="1">
+    <row r="17" spans="2:8" ht="408.75" customHeight="1">
       <c r="B17" s="19" t="s">
         <v>31</v>
       </c>
@@ -12412,7 +12454,7 @@
         <v>240</v>
       </c>
       <c r="D17" s="47" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Updated timesheet and location page
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59C30DC1-1F5E-466E-A3DD-5BAC07469400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{384F3761-3DBC-438A-B925-23C459AEAFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="15" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
     <sheet name="Day15 ( 23-04-2022 )" sheetId="54" r:id="rId13"/>
     <sheet name="Day16 (25-04-2022) (2)" sheetId="58" r:id="rId14"/>
     <sheet name="Day17(26-04-2022)" sheetId="57" r:id="rId15"/>
-    <sheet name="Day18(27-04-2022)  (2)" sheetId="61" r:id="rId16"/>
+    <sheet name="Day18(27-04-2022) " sheetId="61" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="274">
   <si>
     <t>Column1</t>
   </si>
@@ -1053,9 +1053,10 @@
     <t>Working on Register screen</t>
   </si>
   <si>
-    <t>8.45 am - 10.45 am : Corrections done in Data model and Prototype
+    <t xml:space="preserve">8.45 am - 10.45 am : Corrections done in Data model and Prototype
 11.15 am - 12.45 pm : register layout
-1.15 pm - 2.30 pm : Refined Services(Role, Department, Employee, Drive, Pool, Location)</t>
+1.15 pm - 2.30 pm : Refined Services(Role, Department, Employee, Drive, Pool, Location)                                    3.00 to 3.45 : Review Meeting with Rafi
+4.20 to 4.40 : Session with Rafi (Estimation)             5.00pm to 5.30pm : worked on comman layout                                                     5.45 to 6.00 : Meeting with team members(Common Layout).                                                                                           </t>
   </si>
   <si>
     <t>Should focus on Angular and Interactions</t>
@@ -1172,10 +1173,19 @@
 12.00 to 1.00 : Listing down the API usage for particular pages for reuse and Estimation</t>
   </si>
   <si>
-    <t>Yesterday:                                                                            3.00 to 3.45 : Review Meeting with Rafi
-4.20 to 4.40 : Session with Rafi (Estimation)             5.00pm to 5.30pm : worked on comman layout                                                     5.45 to 6.00 : Meeting with team members(Common Layout).                                                                                           Today:                                                                                              8.45 am - 9.30 am : worked on Login page 
+    <t>Working on Common layout</t>
+  </si>
+  <si>
+    <t>8.45 am - 9.30 am : worked on Login page 
 9.45 am - 10.30 am : Soft skill Session with savitha
-11.00 am - 12.30 pm : worked on register page</t>
+11.00 am - 12.30 pm : worked on register page 
+1.30 pm - 2.30 pm :Worked on Common Layout page
+2.30 pm - 2.50 pm : Review with rafi
+3.10 pm - 3.30 : Team Meeting
+3.30 - 4.00 : Worked on common layout page
+4.30 - 5.45 :Worked on common layout page
+7.00 - 8.00 : completed common layout page
+9.00 - 11.00 : Worked on current drives, home, profile, view response</t>
   </si>
   <si>
     <t xml:space="preserve">Should focus on Layout </t>
@@ -1268,7 +1278,7 @@
 8.00 to 9.00 : Worked on Most reused API &amp; Operation for Priority.</t>
   </si>
   <si>
-    <t>Vinoth (TL)</t>
+    <t>Vinoth J</t>
   </si>
   <si>
     <t xml:space="preserve">8.45 am  -  9.00 am : checking mails
@@ -12598,322 +12608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF485B7A-AA69-4806-81E2-DF87DCB7E7C5}">
   <dimension ref="A4:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="57.28515625" customWidth="1"/>
-    <col min="3" max="3" width="72.28515625" customWidth="1"/>
-    <col min="4" max="5" width="70.42578125" customWidth="1"/>
-    <col min="6" max="6" width="72.7109375" customWidth="1"/>
-    <col min="7" max="7" width="82.28515625" customWidth="1"/>
-    <col min="8" max="8" width="109.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="1:8" ht="42">
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" ht="105">
-      <c r="B5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="21">
-      <c r="B6" s="6"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" ht="21">
-      <c r="B7" s="4"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" ht="20.25">
-      <c r="B8" s="11"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" ht="105">
-      <c r="A9" s="12"/>
-      <c r="B9" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="165.75">
-      <c r="B10" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="35" t="s">
-        <v>228</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="35">
-        <v>1</v>
-      </c>
-      <c r="G10" s="35">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H10" s="23"/>
-    </row>
-    <row r="11" spans="1:8" ht="224.25" customHeight="1">
-      <c r="B11" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>218</v>
-      </c>
-      <c r="D11" s="47" t="s">
-        <v>230</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="35">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G11" s="35" t="s">
-        <v>214</v>
-      </c>
-      <c r="H11" s="24"/>
-    </row>
-    <row r="12" spans="1:8" ht="177.75" customHeight="1">
-      <c r="B12" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="35" t="s">
-        <v>231</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="35">
-        <v>2.15</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>217</v>
-      </c>
-      <c r="H12" s="24"/>
-    </row>
-    <row r="13" spans="1:8" ht="186.75" customHeight="1">
-      <c r="B13" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>233</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="35">
-        <v>2.5</v>
-      </c>
-      <c r="G13" s="35" t="s">
-        <v>217</v>
-      </c>
-      <c r="H13" s="25"/>
-    </row>
-    <row r="14" spans="1:8" ht="248.25" customHeight="1">
-      <c r="B14" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="35" t="s">
-        <v>235</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="25"/>
-    </row>
-    <row r="15" spans="1:8" ht="211.5" customHeight="1">
-      <c r="B15" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="D15" s="44" t="s">
-        <v>238</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="35">
-        <v>4</v>
-      </c>
-      <c r="G15" s="35">
-        <v>0</v>
-      </c>
-      <c r="H15" s="25"/>
-    </row>
-    <row r="16" spans="1:8" ht="204" customHeight="1">
-      <c r="B16" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="35" t="s">
-        <v>167</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="35">
-        <v>3</v>
-      </c>
-      <c r="G16" s="35">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="H16" s="25"/>
-    </row>
-    <row r="17" spans="2:8" ht="232.5" customHeight="1">
-      <c r="B17" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>240</v>
-      </c>
-      <c r="D17" s="47" t="s">
-        <v>241</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="45">
-        <v>3</v>
-      </c>
-      <c r="G17" s="35" t="s">
-        <v>208</v>
-      </c>
-      <c r="H17" s="26"/>
-    </row>
-    <row r="18" spans="2:8" ht="207.75" customHeight="1">
-      <c r="B18" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>242</v>
-      </c>
-      <c r="D18" s="44" t="s">
-        <v>243</v>
-      </c>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35">
-        <v>4</v>
-      </c>
-      <c r="G18" s="35">
-        <v>0</v>
-      </c>
-      <c r="H18" s="27"/>
-    </row>
-    <row r="19" spans="2:8" ht="208.5" customHeight="1">
-      <c r="B19" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="37" t="s">
-        <v>244</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>245</v>
-      </c>
-      <c r="E19" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="42">
-        <v>4.5</v>
-      </c>
-      <c r="G19" s="42">
-        <v>2.5</v>
-      </c>
-      <c r="H19" s="28"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7B8EE2-C09E-4672-919D-0F2EB56C51A0}">
-  <dimension ref="A4:H19"/>
-  <sheetViews>
-    <sheetView topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13011,7 +12707,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="331.5">
+    <row r="10" spans="1:8" ht="165.75">
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
@@ -13019,7 +12715,7 @@
         <v>228</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="E10" s="35" t="s">
         <v>41</v>
@@ -13032,49 +12728,49 @@
       </c>
       <c r="H10" s="23"/>
     </row>
-    <row r="11" spans="1:8" ht="348" customHeight="1">
+    <row r="11" spans="1:8" ht="224.25" customHeight="1">
       <c r="B11" s="19" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>247</v>
+        <v>218</v>
       </c>
       <c r="D11" s="47" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="E11" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F11" s="35">
-        <v>4</v>
-      </c>
-      <c r="G11" s="35">
-        <v>1.5</v>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>214</v>
       </c>
       <c r="H11" s="24"/>
     </row>
-    <row r="12" spans="1:8" ht="327.75" customHeight="1">
+    <row r="12" spans="1:8" ht="177.75" customHeight="1">
       <c r="B12" s="19" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>160</v>
+        <v>231</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="E12" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="35">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="G12" s="35">
-        <v>1</v>
+        <v>2.15</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>217</v>
       </c>
       <c r="H12" s="24"/>
     </row>
-    <row r="13" spans="1:8" ht="230.25" customHeight="1">
+    <row r="13" spans="1:8" ht="186.75" customHeight="1">
       <c r="B13" s="19" t="s">
         <v>21</v>
       </c>
@@ -13082,7 +12778,7 @@
         <v>233</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>41</v>
@@ -13103,7 +12799,7 @@
         <v>235</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="E14" s="35" t="s">
         <v>41</v>
@@ -13112,15 +12808,15 @@
       <c r="G14" s="35"/>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="329.25" customHeight="1">
+    <row r="15" spans="1:8" ht="211.5" customHeight="1">
       <c r="B15" s="19" t="s">
         <v>27</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="D15" s="44" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
@@ -13133,7 +12829,7 @@
       </c>
       <c r="H15" s="25"/>
     </row>
-    <row r="16" spans="1:8" ht="395.25" customHeight="1">
+    <row r="16" spans="1:8" ht="204" customHeight="1">
       <c r="B16" s="19" t="s">
         <v>30</v>
       </c>
@@ -13141,7 +12837,7 @@
         <v>167</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>41</v>
@@ -13154,7 +12850,7 @@
       </c>
       <c r="H16" s="25"/>
     </row>
-    <row r="17" spans="2:8" ht="409.5" customHeight="1">
+    <row r="17" spans="2:8" ht="232.5" customHeight="1">
       <c r="B17" s="19" t="s">
         <v>31</v>
       </c>
@@ -13162,7 +12858,7 @@
         <v>240</v>
       </c>
       <c r="D17" s="47" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>41</v>
@@ -13175,7 +12871,7 @@
       </c>
       <c r="H17" s="26"/>
     </row>
-    <row r="18" spans="2:8" ht="291.75" customHeight="1">
+    <row r="18" spans="2:8" ht="207.75" customHeight="1">
       <c r="B18" s="19" t="s">
         <v>34</v>
       </c>
@@ -13183,14 +12879,14 @@
         <v>242</v>
       </c>
       <c r="D18" s="44" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="E18" s="35"/>
       <c r="F18" s="35">
-        <v>5</v>
-      </c>
-      <c r="G18" s="35" t="s">
-        <v>217</v>
+        <v>4</v>
+      </c>
+      <c r="G18" s="35">
+        <v>0</v>
       </c>
       <c r="H18" s="27"/>
     </row>
@@ -13199,10 +12895,10 @@
         <v>54</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="E19" s="35" t="s">
         <v>41</v>
@@ -13224,12 +12920,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7E5E1D-E354-4FCD-AD92-53A00E511336}">
-  <dimension ref="A4:H21"/>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7B8EE2-C09E-4672-919D-0F2EB56C51A0}">
+  <dimension ref="A4:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13348,6 +13044,322 @@
       </c>
       <c r="H10" s="23"/>
     </row>
+    <row r="11" spans="1:8" ht="348" customHeight="1">
+      <c r="B11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>248</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="35">
+        <v>4</v>
+      </c>
+      <c r="G11" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12" spans="1:8" ht="327.75" customHeight="1">
+      <c r="B12" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="35">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G12" s="35">
+        <v>1</v>
+      </c>
+      <c r="H12" s="24"/>
+    </row>
+    <row r="13" spans="1:8" ht="230.25" customHeight="1">
+      <c r="B13" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="35">
+        <v>2.5</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="1:8" ht="248.25" customHeight="1">
+      <c r="B14" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="25"/>
+    </row>
+    <row r="15" spans="1:8" ht="329.25" customHeight="1">
+      <c r="B15" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="35">
+        <v>4</v>
+      </c>
+      <c r="G15" s="35">
+        <v>0</v>
+      </c>
+      <c r="H15" s="25"/>
+    </row>
+    <row r="16" spans="1:8" ht="395.25" customHeight="1">
+      <c r="B16" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="35">
+        <v>3</v>
+      </c>
+      <c r="G16" s="35">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H16" s="25"/>
+    </row>
+    <row r="17" spans="2:8" ht="409.5" customHeight="1">
+      <c r="B17" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>255</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="45">
+        <v>3</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="H17" s="26"/>
+    </row>
+    <row r="18" spans="2:8" ht="291.75" customHeight="1">
+      <c r="B18" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35">
+        <v>9.25</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="H18" s="27"/>
+    </row>
+    <row r="19" spans="2:8" ht="208.5" customHeight="1">
+      <c r="B19" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>259</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="42">
+        <v>4.5</v>
+      </c>
+      <c r="G19" s="42">
+        <v>2.5</v>
+      </c>
+      <c r="H19" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7E5E1D-E354-4FCD-AD92-53A00E511336}">
+  <dimension ref="A4:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="57.28515625" customWidth="1"/>
+    <col min="3" max="3" width="72.28515625" customWidth="1"/>
+    <col min="4" max="5" width="70.42578125" customWidth="1"/>
+    <col min="6" max="6" width="72.7109375" customWidth="1"/>
+    <col min="7" max="7" width="82.28515625" customWidth="1"/>
+    <col min="8" max="8" width="109.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:8" ht="42">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="105">
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="21">
+      <c r="B6" s="6"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="21">
+      <c r="B7" s="4"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="20.25">
+      <c r="B8" s="11"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="105">
+      <c r="A9" s="12"/>
+      <c r="B9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="331.5">
+      <c r="B10" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="35">
+        <v>1</v>
+      </c>
+      <c r="G10" s="35">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H10" s="23"/>
+    </row>
     <row r="11" spans="1:8" ht="120.75" customHeight="1">
       <c r="B11" s="19" t="s">
         <v>17</v>
@@ -13356,7 +13368,7 @@
         <v>73</v>
       </c>
       <c r="D11" s="47" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E11" s="35" t="s">
         <v>41</v>
@@ -13367,13 +13379,13 @@
     </row>
     <row r="12" spans="1:8" ht="373.5" customHeight="1">
       <c r="B12" s="19" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E12" s="35" t="s">
         <v>41</v>
@@ -13394,7 +13406,7 @@
         <v>73</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>41</v>
@@ -13422,13 +13434,13 @@
     </row>
     <row r="15" spans="1:8" ht="405" customHeight="1">
       <c r="B15" s="19" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D15" s="44" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
@@ -13449,7 +13461,7 @@
         <v>167</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>41</v>
@@ -13464,13 +13476,13 @@
     </row>
     <row r="17" spans="2:8" ht="409.5" customHeight="1">
       <c r="B17" s="19" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E17" s="35"/>
       <c r="F17" s="35">
@@ -13481,12 +13493,18 @@
     </row>
     <row r="18" spans="2:8" ht="336" customHeight="1">
       <c r="B18" s="19" t="s">
-        <v>271</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="13"/>
+        <v>272</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>257</v>
+      </c>
       <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
+      <c r="F18" s="35">
+        <v>9.25</v>
+      </c>
       <c r="G18" s="35"/>
       <c r="H18" s="25"/>
     </row>
@@ -13498,7 +13516,7 @@
         <v>41</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E19" s="35" t="s">
         <v>41</v>

</xml_diff>